<commit_message>
Essential changes to datasets
</commit_message>
<xml_diff>
--- a/data 10.xlsx
+++ b/data 10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurg/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stijn\Documents\GitHub\Storytelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241262CD-F3C1-5E4F-B810-8AC7231BDAC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20FB78B-EE1D-4BEC-BD25-8177F2BDB704}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15600" xr2:uid="{20B37368-0FA3-854A-9616-351CBED4ACF4}"/>
+    <workbookView xWindow="28644" yWindow="-7128" windowWidth="24348" windowHeight="19068" xr2:uid="{20B37368-0FA3-854A-9616-351CBED4ACF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,19 +39,19 @@
     <t>Delivery window (hours)</t>
   </si>
   <si>
-    <t>Mono Packaging Materials</t>
+    <t>A Mono Packaging Materials</t>
   </si>
   <si>
-    <t>Trio PET PLC</t>
+    <t>B Trio PET PLC</t>
   </si>
   <si>
-    <t>Miami Oranges</t>
+    <t>C Miami Oranges</t>
   </si>
   <si>
-    <t>NO8DO Mango</t>
+    <t>D NO8DO Mango</t>
   </si>
   <si>
-    <t>Seitan Vitamins</t>
+    <t>E Seitan Vitamins</t>
   </si>
 </sst>
 </file>
@@ -441,18 +432,18 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +457,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5">
@@ -480,8 +471,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5">
@@ -494,8 +485,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5">
@@ -508,8 +499,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5">
@@ -522,8 +513,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5">
@@ -536,7 +527,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -550,7 +541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -564,7 +555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -578,7 +569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -592,7 +583,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -606,7 +597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -620,7 +611,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -634,7 +625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -648,7 +639,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -662,7 +653,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -676,7 +667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -690,7 +681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -704,7 +695,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -718,7 +709,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -732,7 +723,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -746,7 +737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
@@ -760,7 +751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
@@ -774,7 +765,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -788,7 +779,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
@@ -802,7 +793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>